<commit_message>
Update Positive Development Network
</commit_message>
<xml_diff>
--- a/Positive Development/Analyses/Other/mutate_shortcut.xlsx
+++ b/Positive Development/Analyses/Other/mutate_shortcut.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5092CE46-2EA6-48CA-9E55-89A1F5B94A3D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CBE7718-7FAB-48F5-80B9-BD3D0F5001C8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Start" sheetId="1" r:id="rId1"/>
@@ -455,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1358,8 +1358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63DDF13F-C4B2-4E2F-BFD7-4E2793A35067}">
   <dimension ref="A1:A32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>